<commit_message>
a script to collect results
</commit_message>
<xml_diff>
--- a/intdiv.xlsx
+++ b/intdiv.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozgurakgun/repos/github/ozgurakgun/magic-hexagon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D9E1C5-6182-274F-B17E-B9A077B8B78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503C7A66-E96C-1440-8402-3EBC12F25EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23500" yWindow="15060" windowWidth="22380" windowHeight="28140" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
+    <workbookView xWindow="45160" yWindow="9220" windowWidth="22380" windowHeight="28140" activeTab="1" xr2:uid="{81ED7F14-820B-C144-81AC-28F30AD4118D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Order</t>
   </si>
@@ -51,6 +52,33 @@
   </si>
   <si>
     <t>Per "row"</t>
+  </si>
+  <si>
+    <t>Time limit</t>
+  </si>
+  <si>
+    <t>Chuffed</t>
+  </si>
+  <si>
+    <t>Kissat</t>
+  </si>
+  <si>
+    <t>OR-Tools</t>
+  </si>
+  <si>
+    <t>1 minute</t>
+  </si>
+  <si>
+    <t>10 seconds</t>
+  </si>
+  <si>
+    <t>5 minutes</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Number of instances solved</t>
   </si>
 </sst>
 </file>
@@ -86,8 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5808C9C4-3E6C-2C41-BE4F-8BFC865CE1AA}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -640,4 +671,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2880405E-5811-F449-AB85-0B9EC024ACDD}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>